<commit_message>
add allergyintolerance and observation profiles
</commit_message>
<xml_diff>
--- a/StructureDefinition-be-mycarenetclaim.xlsx
+++ b/StructureDefinition-be-mycarenetclaim.xlsx
@@ -1201,7 +1201,7 @@
     <t>Typically these information codes are required to support the services rendered or the adjudication of the services rendered.</t>
   </si>
   <si>
-    <t xml:space="preserve">value:system}
+    <t xml:space="preserve">value:category.coding.code}
 </t>
   </si>
   <si>
@@ -2486,7 +2486,7 @@
     <col min="24" max="24" width="121.30859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="70.8671875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="26.2890625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="43.01953125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
@@ -11528,7 +11528,7 @@
       </c>
       <c r="D84" s="2"/>
       <c r="E84" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F84" t="s" s="2">
         <v>50</v>
@@ -13918,7 +13918,7 @@
       </c>
       <c r="D106" s="2"/>
       <c r="E106" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F106" t="s" s="2">
         <v>50</v>

</xml_diff>